<commit_message>
cleaned up some code, added support for reading thermistors, but need a convertiontable to get readouts in degrees
</commit_message>
<xml_diff>
--- a/PCB_rev1/Replicape_BOM_rev1.xlsx
+++ b/PCB_rev1/Replicape_BOM_rev1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
   <si>
     <t>Digikey Part nr. </t>
   </si>
@@ -309,6 +309,12 @@
   </si>
   <si>
     <t>P8-RECEPTABLE</t>
+  </si>
+  <si>
+    <t>296-9544-1-ND</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 1.2MHZ QUAD 14TSSOP</t>
   </si>
   <si>
     <t>Price each</t>
@@ -351,7 +357,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +374,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFFF00"/>
         <bgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0033CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -405,7 +417,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -422,6 +434,11 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
@@ -500,10 +517,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A31" activeCellId="0" pane="topLeft" sqref="A31"/>
+      <selection activeCell="A34" activeCellId="0" pane="topLeft" sqref="A34:I34"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -1506,26 +1523,35 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
-      <c r="A33" s="8" t="s">
+      <c r="A32" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8" t="n">
+      <c r="B32" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+      <c r="A34" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11" t="n">
         <f aca="false">SUM(F2:F31)</f>
         <v>87.547</v>
       </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8" t="n">
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11" t="n">
         <f aca="false">SUM(I2:I31)/500</f>
         <v>44.38788</v>
       </c>

</xml_diff>

<commit_message>
renamed folder misspelling for literature. Added BeagleBone as optional on Rev1 BOM
</commit_message>
<xml_diff>
--- a/PCB_rev1/Replicape_BOM_rev1.xlsx
+++ b/PCB_rev1/Replicape_BOM_rev1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
   <si>
     <t>Digikey Part nr.</t>
   </si>
@@ -327,6 +327,15 @@
   </si>
   <si>
     <t>Price each</t>
+  </si>
+  <si>
+    <t>Optional:</t>
+  </si>
+  <si>
+    <t>KIT BEAGLEBONE DEV</t>
+  </si>
+  <si>
+    <t>NONE</t>
   </si>
 </sst>
 </file>
@@ -536,19 +545,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F38" activeCellId="0" pane="topLeft" sqref="F38"/>
+      <selection activeCell="A40" activeCellId="0" pane="topLeft" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.3921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.4941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6705882352941"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>9</v>
       </c>
@@ -609,7 +618,7 @@
         <v>113.04</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
@@ -641,7 +650,7 @@
         <v>85.995</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>15</v>
       </c>
@@ -673,7 +682,7 @@
         <v>34.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>18</v>
       </c>
@@ -705,7 +714,7 @@
         <v>197.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>21</v>
       </c>
@@ -737,7 +746,7 @@
         <v>416</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>24</v>
       </c>
@@ -769,7 +778,7 @@
         <v>1844.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -800,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
@@ -832,7 +841,7 @@
         <v>384.75</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -864,7 +873,7 @@
         <v>216.51</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>36</v>
       </c>
@@ -896,7 +905,7 @@
         <v>8156.25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>39</v>
       </c>
@@ -928,7 +937,7 @@
         <v>877.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>42</v>
       </c>
@@ -960,7 +969,7 @@
         <v>665</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="5" t="s">
         <v>45</v>
       </c>
@@ -992,7 +1001,7 @@
         <v>177.68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>48</v>
       </c>
@@ -1024,7 +1033,7 @@
         <v>2331.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>51</v>
       </c>
@@ -1056,7 +1065,7 @@
         <v>331.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>54</v>
       </c>
@@ -1088,7 +1097,7 @@
         <v>3.555</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>57</v>
       </c>
@@ -1120,7 +1129,7 @@
         <v>18.69</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>60</v>
       </c>
@@ -1152,7 +1161,7 @@
         <v>900.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>63</v>
       </c>
@@ -1184,7 +1193,7 @@
         <v>519.75</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>66</v>
       </c>
@@ -1216,7 +1225,7 @@
         <v>892.11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>69</v>
       </c>
@@ -1248,7 +1257,7 @@
         <v>391.23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>72</v>
       </c>
@@ -1280,7 +1289,7 @@
         <v>108</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
         <v>74</v>
       </c>
@@ -1312,7 +1321,7 @@
         <v>115.96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
         <v>77</v>
       </c>
@@ -1344,7 +1353,7 @@
         <v>45.3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
         <v>80</v>
       </c>
@@ -1376,7 +1385,7 @@
         <v>12.15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
         <v>83</v>
       </c>
@@ -1408,7 +1417,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>86</v>
       </c>
@@ -1440,7 +1449,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="4" t="s">
         <v>89</v>
       </c>
@@ -1472,7 +1481,7 @@
         <v>349.47</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="5" t="s">
         <v>92</v>
       </c>
@@ -1503,7 +1512,7 @@
         <v>2749.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="3" t="s">
         <v>95</v>
       </c>
@@ -1534,7 +1543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="8" t="s">
         <v>98</v>
       </c>
@@ -1563,7 +1572,7 @@
         <v>80.28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="12" t="s">
         <v>100</v>
       </c>
@@ -1594,7 +1603,7 @@
         <v>167.48</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="13" t="s">
         <v>103</v>
       </c>
@@ -1611,6 +1620,28 @@
       <c r="I34" s="13" t="n">
         <f aca="false">SUM(I2:I33)/500</f>
         <v>44.5572</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+      <c r="A36" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+      <c r="A37" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First commit after makeing it work for Rev 1.
</commit_message>
<xml_diff>
--- a/PCB_rev1/Replicape_BOM_rev1.xlsx
+++ b/PCB_rev1/Replicape_BOM_rev1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="110">
   <si>
     <t>Digikey Part nr.</t>
   </si>
@@ -59,7 +59,7 @@
     <t>CONN HEADER RTANG 3POS .100 TIN</t>
   </si>
   <si>
-    <t>X10, X11, X12</t>
+    <t>X10, X11, X12, X1, X13, X19</t>
   </si>
   <si>
     <t>S9338-ND</t>
@@ -107,10 +107,10 @@
     <t>X2-2</t>
   </si>
   <si>
-    <t>WM6988-ND</t>
-  </si>
-  <si>
-    <t>CONN HEADER 4POS .200 RT ANG TIN</t>
+    <t>281-2845-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER 4POS 5.08MM R/A</t>
   </si>
   <si>
     <t>X2</t>
@@ -185,7 +185,7 @@
     <t>RES 4.7K OHM 1/16W 5% 0402 SMD</t>
   </si>
   <si>
-    <t>R13, R17, R18</t>
+    <t>R13, R17, R18, R38, R39</t>
   </si>
   <si>
     <t>311-1.0KJRCT-ND</t>
@@ -206,6 +206,15 @@
     <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10</t>
   </si>
   <si>
+    <t>P5.6KJCT-ND</t>
+  </si>
+  <si>
+    <t>RES 5.6K OHM 1/10W 5% 0402 SMD</t>
+  </si>
+  <si>
+    <t>R22, R23, R24</t>
+  </si>
+  <si>
     <t>NIF5002NT3GOSCT-ND</t>
   </si>
   <si>
@@ -263,16 +272,13 @@
     <t>CAP CER 0.1UF 25V Y5V 0402</t>
   </si>
   <si>
-    <t>C11, C13, C17, C20, C22, C24</t>
-  </si>
-  <si>
     <t>311-1363-1-ND</t>
   </si>
   <si>
     <t>CAP CER 0.1UF 25V 20% Y5V 0603</t>
   </si>
   <si>
-    <t>C2, C4, C6, C8, C10, C19, C29, C31, C33, C35, C3</t>
+    <t>C2, C4, C6, C8, C10, C19, C29, C31, C33, C35, C3, C11, C13, C17, C20, C22, C24</t>
   </si>
   <si>
     <t>311-1360-1-ND</t>
@@ -290,7 +296,7 @@
     <t>CONN HEADER .100 DUAL STR 26POS</t>
   </si>
   <si>
-    <t>P8-PIN</t>
+    <t> </t>
   </si>
   <si>
     <t>SAM1204-23-ND</t>
@@ -299,7 +305,7 @@
     <t>CONN RCPT .100" 46POS DUAL TIN</t>
   </si>
   <si>
-    <t>P9-EXPANSION_A</t>
+    <t>P9-EXPANSION_A, P8-EXPANSION_A</t>
   </si>
   <si>
     <t>SAM1204-10-ND</t>
@@ -308,13 +314,13 @@
     <t>CONN RCPT .100" 20POS DUAL TIN</t>
   </si>
   <si>
-    <t>P8-RECEPTABLE</t>
-  </si>
-  <si>
-    <t>296-9544-1-ND</t>
-  </si>
-  <si>
-    <t>IC OPAMP GP 1.2MHZ QUAD 14TSSOP</t>
+    <t>296-6604-1-ND</t>
+  </si>
+  <si>
+    <t>IC QUAD DIFF COMPARATOR 14 -SOIC</t>
+  </si>
+  <si>
+    <t>IC1</t>
   </si>
   <si>
     <t>PCE3917CT-ND</t>
@@ -336,6 +342,9 @@
   </si>
   <si>
     <t>NONE</t>
+  </si>
+  <si>
+    <t>Alt:</t>
   </si>
 </sst>
 </file>
@@ -384,12 +393,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00FFFF00"/>
         <bgColor rgb="00FFFF00"/>
       </patternFill>
@@ -398,6 +401,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="0000FF00"/>
         <bgColor rgb="0023FF23"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00993300"/>
       </patternFill>
     </fill>
     <fill>
@@ -441,7 +450,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -453,16 +462,21 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
@@ -545,16 +559,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A40" activeCellId="0" pane="topLeft" sqref="A40"/>
+      <selection activeCell="C32" activeCellId="0" pane="topLeft" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5647058823529"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.4941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6705882352941"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6274509803922"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.5960784313725"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7098039215686"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -619,35 +633,35 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="n">
+      <c r="D3" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="n">
         <v>0.14</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="4" t="n">
         <f aca="false">D3*E3</f>
-        <v>0.42</v>
-      </c>
-      <c r="G3" s="2" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="G3" s="4" t="n">
         <f aca="false">D3*500</f>
-        <v>1500</v>
-      </c>
-      <c r="H3" s="2" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H3" s="4" t="n">
         <v>0.05733</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" s="4" t="n">
         <f aca="false">G3*H3</f>
-        <v>85.995</v>
+        <v>171.99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
@@ -779,41 +793,41 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <f aca="false">D8*E8</f>
+        <v>2.5</v>
+      </c>
+      <c r="G8" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F8" s="4" t="n">
-        <f aca="false">D8*E8</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="4" t="n">
+      <c r="H8" s="6" t="n">
         <v>1.7</v>
       </c>
-      <c r="I8" s="4" t="n">
+      <c r="I8" s="6" t="n">
         <f aca="false">G8*H8</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -822,53 +836,53 @@
       <c r="D9" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="5" t="n">
-        <v>1.24</v>
+      <c r="E9" s="6" t="n">
+        <v>1.32</v>
       </c>
       <c r="F9" s="6" t="n">
         <f aca="false">D9*E9</f>
-        <v>1.24</v>
+        <v>1.32</v>
       </c>
       <c r="G9" s="6" t="n">
         <f aca="false">D9*500</f>
         <v>500</v>
       </c>
-      <c r="H9" s="5" t="n">
-        <v>0.7695</v>
+      <c r="H9" s="6" t="n">
+        <v>0.924</v>
       </c>
       <c r="I9" s="6" t="n">
         <f aca="false">G9*H9</f>
-        <v>384.75</v>
+        <v>462</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="D10" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="6" t="n">
+      <c r="E10" s="4" t="n">
         <v>0.6</v>
       </c>
-      <c r="F10" s="6" t="n">
+      <c r="F10" s="4" t="n">
         <f aca="false">D10*E10</f>
         <v>0.6</v>
       </c>
-      <c r="G10" s="6" t="n">
+      <c r="G10" s="4" t="n">
         <f aca="false">D10*500</f>
         <v>500</v>
       </c>
-      <c r="H10" s="6" t="n">
+      <c r="H10" s="4" t="n">
         <v>0.43302</v>
       </c>
-      <c r="I10" s="6" t="n">
+      <c r="I10" s="4" t="n">
         <f aca="false">G10*H10</f>
         <v>216.51</v>
       </c>
@@ -970,33 +984,33 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D14" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="6" t="n">
+      <c r="E14" s="4" t="n">
         <v>0.71</v>
       </c>
-      <c r="F14" s="6" t="n">
+      <c r="F14" s="4" t="n">
         <f aca="false">D14*E14</f>
         <v>0.71</v>
       </c>
-      <c r="G14" s="6" t="n">
+      <c r="G14" s="4" t="n">
         <f aca="false">D14*500</f>
         <v>500</v>
       </c>
-      <c r="H14" s="5" t="n">
+      <c r="H14" s="3" t="n">
         <v>0.35536</v>
       </c>
-      <c r="I14" s="6" t="n">
+      <c r="I14" s="4" t="n">
         <f aca="false">G14*H14</f>
         <v>177.68</v>
       </c>
@@ -1066,35 +1080,35 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E17" s="2" t="n">
+      <c r="D17" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="4" t="n">
         <f aca="false">D17*E17</f>
-        <v>0.3</v>
-      </c>
-      <c r="G17" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="4" t="n">
         <f aca="false">D17*500</f>
-        <v>1500</v>
-      </c>
-      <c r="H17" s="2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H17" s="4" t="n">
         <v>0.00237</v>
       </c>
-      <c r="I17" s="2" t="n">
+      <c r="I17" s="4" t="n">
         <f aca="false">G17*H17</f>
-        <v>3.555</v>
+        <v>5.925</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
@@ -1162,35 +1176,34 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="D20" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="E20" s="2" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="F20" s="2" t="n">
+      <c r="E20" s="8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F20" s="8" t="n">
         <f aca="false">D20*E20</f>
-        <v>2.61</v>
-      </c>
-      <c r="G20" s="2" t="n">
-        <f aca="false">D20*500</f>
+        <v>0.3</v>
+      </c>
+      <c r="G20" s="8" t="n">
         <v>1500</v>
       </c>
-      <c r="H20" s="2" t="n">
-        <v>0.3465</v>
-      </c>
-      <c r="I20" s="2" t="n">
+      <c r="H20" s="8" t="n">
+        <v>0.0072</v>
+      </c>
+      <c r="I20" s="8" t="n">
         <f aca="false">G20*H20</f>
-        <v>519.75</v>
+        <v>10.8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
@@ -1207,22 +1220,22 @@
         <v>3</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>1.59</v>
+        <v>0.87</v>
       </c>
       <c r="F21" s="2" t="n">
         <f aca="false">D21*E21</f>
-        <v>4.77</v>
+        <v>2.61</v>
       </c>
       <c r="G21" s="2" t="n">
         <f aca="false">D21*500</f>
         <v>1500</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>0.59474</v>
+        <v>0.3465</v>
       </c>
       <c r="I21" s="2" t="n">
         <f aca="false">G21*H21</f>
-        <v>892.11</v>
+        <v>519.75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
@@ -1236,25 +1249,25 @@
         <v>71</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>0.21</v>
+        <v>1.59</v>
       </c>
       <c r="F22" s="2" t="n">
         <f aca="false">D22*E22</f>
-        <v>1.47</v>
+        <v>4.77</v>
       </c>
       <c r="G22" s="2" t="n">
         <f aca="false">D22*500</f>
-        <v>3500</v>
+        <v>1500</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>0.11178</v>
+        <v>0.59474</v>
       </c>
       <c r="I22" s="2" t="n">
         <f aca="false">G22*H22</f>
-        <v>391.23</v>
+        <v>892.11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
@@ -1265,60 +1278,60 @@
         <v>73</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>0.16</v>
+        <v>0.21</v>
       </c>
       <c r="F23" s="2" t="n">
         <f aca="false">D23*E23</f>
-        <v>0.48</v>
+        <v>1.47</v>
       </c>
       <c r="G23" s="2" t="n">
         <f aca="false">D23*500</f>
-        <v>1500</v>
+        <v>3500</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>0.072</v>
+        <v>0.11178</v>
       </c>
       <c r="I23" s="2" t="n">
         <f aca="false">G23*H23</f>
-        <v>108</v>
+        <v>391.23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="F24" s="2" t="n">
         <f aca="false">D24*E24</f>
-        <v>1.2</v>
+        <v>0.48</v>
       </c>
       <c r="G24" s="2" t="n">
         <f aca="false">D24*500</f>
-        <v>4000</v>
+        <v>1500</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>0.02899</v>
+        <v>0.072</v>
       </c>
       <c r="I24" s="2" t="n">
         <f aca="false">G24*H24</f>
-        <v>115.96</v>
+        <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
@@ -1332,25 +1345,25 @@
         <v>79</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F25" s="2" t="n">
         <f aca="false">D25*E25</f>
-        <v>0.48</v>
+        <v>1.2</v>
       </c>
       <c r="G25" s="2" t="n">
         <f aca="false">D25*500</f>
-        <v>1500</v>
+        <v>4000</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>0.0302</v>
+        <v>0.02899</v>
       </c>
       <c r="I25" s="2" t="n">
         <f aca="false">G25*H25</f>
-        <v>45.3</v>
+        <v>115.96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
@@ -1364,284 +1377,321 @@
         <v>82</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
       <c r="F26" s="2" t="n">
         <f aca="false">D26*E26</f>
-        <v>0.6</v>
+        <v>0.48</v>
       </c>
       <c r="G26" s="2" t="n">
         <f aca="false">D26*500</f>
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>0.00405</v>
+        <v>0.0302</v>
       </c>
       <c r="I26" s="2" t="n">
         <f aca="false">G26*H26</f>
-        <v>12.15</v>
+        <v>45.3</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="10"/>
+      <c r="D27" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="10" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F27" s="10" t="n">
+        <f aca="false">D27*E27</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="10" t="n">
+        <f aca="false">D27*500</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="10" t="n">
+        <v>0.00405</v>
+      </c>
+      <c r="I27" s="10" t="n">
+        <f aca="false">G27*H27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="A28" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="E27" s="2" t="n">
+      <c r="B28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="E28" s="4" t="n">
         <v>0.041</v>
       </c>
-      <c r="F27" s="2" t="n">
-        <f aca="false">D27*E27</f>
-        <v>0.615</v>
-      </c>
-      <c r="G27" s="2" t="n">
-        <f aca="false">D27*500</f>
-        <v>7500</v>
-      </c>
-      <c r="H27" s="2" t="n">
+      <c r="F28" s="4" t="n">
+        <f aca="false">D28*E28</f>
+        <v>0.861</v>
+      </c>
+      <c r="G28" s="4" t="n">
+        <f aca="false">D28*500</f>
+        <v>10500</v>
+      </c>
+      <c r="H28" s="4" t="n">
         <v>0.0102</v>
       </c>
-      <c r="I27" s="2" t="n">
-        <f aca="false">G27*H27</f>
-        <v>76.5</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
-      <c r="A28" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="I28" s="4" t="n">
+        <f aca="false">G28*H28</f>
+        <v>107.1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="A29" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="2" t="n">
+      <c r="B29" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E28" s="2" t="n">
+      <c r="E29" s="2" t="n">
         <v>0.1</v>
       </c>
-      <c r="F28" s="2" t="n">
-        <f aca="false">D28*E28</f>
+      <c r="F29" s="2" t="n">
+        <f aca="false">D29*E29</f>
         <v>0.5</v>
       </c>
-      <c r="G28" s="2" t="n">
-        <f aca="false">D28*500</f>
+      <c r="G29" s="2" t="n">
+        <f aca="false">D29*500</f>
         <v>2500</v>
       </c>
-      <c r="H28" s="2" t="n">
+      <c r="H29" s="2" t="n">
         <v>0.00648</v>
       </c>
-      <c r="I28" s="2" t="n">
-        <f aca="false">G28*H28</f>
+      <c r="I29" s="2" t="n">
+        <f aca="false">G29*H29</f>
         <v>16.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
-      <c r="A29" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="4" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="A30" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E29" s="4" t="n">
+      <c r="B30" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="10" t="n">
         <v>1.2</v>
       </c>
-      <c r="F29" s="4" t="n">
-        <f aca="false">D29*E29</f>
-        <v>1.2</v>
-      </c>
-      <c r="G29" s="4" t="n">
-        <f aca="false">D29*500</f>
-        <v>500</v>
-      </c>
-      <c r="H29" s="4" t="n">
+      <c r="F30" s="10" t="n">
+        <f aca="false">D30*E30</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="10" t="n">
+        <f aca="false">D30*500</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="10" t="n">
         <v>0.69894</v>
       </c>
-      <c r="I29" s="4" t="n">
-        <f aca="false">G29*H29</f>
-        <v>349.47</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
-      <c r="A30" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D30" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="E30" s="5" t="n">
-        <v>4.72</v>
-      </c>
-      <c r="F30" s="6" t="n">
-        <f aca="false">E30*D30</f>
-        <v>9.44</v>
-      </c>
-      <c r="G30" s="7" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H30" s="5" t="n">
-        <v>2.7492</v>
-      </c>
-      <c r="I30" s="6" t="n">
-        <f aca="false">H30*G30</f>
-        <v>2749.2</v>
+      <c r="I30" s="10" t="n">
+        <f aca="false">G30*H30</f>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="D31" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>2.64</v>
+        <v>4.72</v>
       </c>
       <c r="F31" s="4" t="n">
         <f aca="false">E31*D31</f>
-        <v>0</v>
+        <v>9.44</v>
       </c>
       <c r="G31" s="3" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H31" s="3" t="n">
-        <v>1.5377</v>
+        <v>2.7492</v>
       </c>
       <c r="I31" s="4" t="n">
         <f aca="false">H31*G31</f>
+        <v>2749.2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
+      <c r="A32" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="10" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
-      <c r="A32" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B32" s="8" t="s">
+      <c r="E32" s="9" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="F32" s="10" t="n">
+        <f aca="false">E32*D32</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="9" t="n">
+        <v>1.5377</v>
+      </c>
+      <c r="I32" s="10" t="n">
+        <f aca="false">H32*G32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
+      <c r="A33" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9" t="n">
+      <c r="B33" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="E32" s="10" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="F32" s="11" t="n">
-        <f aca="false">E32*D32</f>
-        <v>0.44</v>
-      </c>
-      <c r="G32" s="10" t="n">
+      <c r="E33" s="11" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="F33" s="12" t="n">
+        <f aca="false">E33*D33</f>
+        <v>0.41</v>
+      </c>
+      <c r="G33" s="11" t="n">
         <v>500</v>
       </c>
-      <c r="H32" s="10" t="n">
-        <v>0.16056</v>
-      </c>
-      <c r="I32" s="11" t="n">
-        <f aca="false">H32*G32</f>
-        <v>80.28</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
-      <c r="A33" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D33" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="E33" s="12" t="n">
-        <v>0.81</v>
-      </c>
-      <c r="F33" s="11" t="n">
-        <f aca="false">E33*D33</f>
-        <v>0.81</v>
-      </c>
-      <c r="G33" s="12" t="n">
-        <v>500</v>
-      </c>
-      <c r="H33" s="12" t="n">
-        <v>0.33496</v>
-      </c>
-      <c r="I33" s="11" t="n">
+      <c r="H33" s="11" t="n">
+        <v>0.15068</v>
+      </c>
+      <c r="I33" s="12" t="n">
         <f aca="false">H33*G33</f>
-        <v>167.48</v>
+        <v>75.34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13" t="n">
-        <f aca="false">SUM(F2:F33)</f>
-        <v>90.877</v>
-      </c>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13" t="n">
-        <f aca="false">SUM(I2:I33)/500</f>
-        <v>44.5572</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
-      <c r="A36" s="13" t="s">
+      <c r="C34" s="13" t="s">
         <v>104</v>
       </c>
+      <c r="D34" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="13" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="F34" s="12" t="n">
+        <f aca="false">E34*D34</f>
+        <v>0.81</v>
+      </c>
+      <c r="G34" s="13" t="n">
+        <v>500</v>
+      </c>
+      <c r="H34" s="13" t="n">
+        <v>0.33496</v>
+      </c>
+      <c r="I34" s="12" t="n">
+        <f aca="false">H34*G34</f>
+        <v>167.48</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
+      <c r="A35" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14" t="n">
+        <f aca="false">SUM(F2:F34)</f>
+        <v>92.793</v>
+      </c>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14" t="n">
+        <f aca="false">SUM(I2:I34)/500</f>
+        <v>44.23811</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
-      <c r="A37" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" s="0" t="s">
+      <c r="A37" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="D37" s="0" t="n">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
+      <c r="A38" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E38" s="0" t="n">
         <v>89</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="40">
+      <c r="A40" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing before going to 3DP weekend : )
</commit_message>
<xml_diff>
--- a/PCB_rev1/Replicape_BOM_rev1.xlsx
+++ b/PCB_rev1/Replicape_BOM_rev1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="111">
   <si>
     <t>Digikey Part nr.</t>
   </si>
@@ -341,10 +341,13 @@
     <t>KIT BEAGLEBONE DEV</t>
   </si>
   <si>
-    <t>NONE</t>
-  </si>
-  <si>
-    <t>Alt:</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t>BB-BONE-LCD3-01-ND</t>
+  </si>
+  <si>
+    <t>BEAGLEBONE LCD3 CAPE</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -482,6 +485,9 @@
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -559,14 +565,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C32" activeCellId="0" pane="topLeft" sqref="C32"/>
+      <selection activeCell="C40" activeCellId="0" pane="topLeft" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6274509803922"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.043137254902"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.5960784313725"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7098039215686"/>
   </cols>
@@ -1689,9 +1695,21 @@
         <v>89</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="40">
-      <c r="A40" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="39">
+      <c r="A39" s="15" t="s">
         <v>109</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>69.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unable to compile the firmware on Ubuntu, so the firmware file is added for now
</commit_message>
<xml_diff>
--- a/PCB_rev1/Replicape_BOM_rev1.xlsx
+++ b/PCB_rev1/Replicape_BOM_rev1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="110">
   <si>
     <t>Digikey Part nr.</t>
   </si>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t>CONN HEADER .100 DUAL STR 26POS</t>
-  </si>
-  <si>
-    <t> </t>
   </si>
   <si>
     <t>SAM1204-23-ND</t>
@@ -453,7 +450,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -466,9 +463,6 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
@@ -568,13 +562,14 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C40" activeCellId="0" pane="topLeft" sqref="C40"/>
+      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.043137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.5960784313725"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7098039215686"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.121568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6980392156863"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -802,29 +797,29 @@
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="6" t="n">
+      <c r="E8" s="2" t="n">
         <v>2.5</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="2" t="n">
         <f aca="false">D8*E8</f>
         <v>2.5</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="H8" s="6" t="n">
+      <c r="H8" s="2" t="n">
         <v>1.7</v>
       </c>
-      <c r="I8" s="6" t="n">
+      <c r="I8" s="2" t="n">
         <f aca="false">G8*H8</f>
         <v>0</v>
       </c>
@@ -833,30 +828,30 @@
       <c r="A9" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="2" t="n">
         <v>1.32</v>
       </c>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="2" t="n">
         <f aca="false">D9*E9</f>
         <v>1.32</v>
       </c>
-      <c r="G9" s="6" t="n">
+      <c r="G9" s="2" t="n">
         <f aca="false">D9*500</f>
         <v>500</v>
       </c>
-      <c r="H9" s="6" t="n">
+      <c r="H9" s="2" t="n">
         <v>0.924</v>
       </c>
-      <c r="I9" s="6" t="n">
+      <c r="I9" s="2" t="n">
         <f aca="false">G9*H9</f>
         <v>462</v>
       </c>
@@ -1182,32 +1177,32 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="8" t="n">
+      <c r="D20" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="E20" s="8" t="n">
+      <c r="E20" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="F20" s="8" t="n">
+      <c r="F20" s="7" t="n">
         <f aca="false">D20*E20</f>
         <v>0.3</v>
       </c>
-      <c r="G20" s="8" t="n">
+      <c r="G20" s="7" t="n">
         <v>1500</v>
       </c>
-      <c r="H20" s="8" t="n">
+      <c r="H20" s="7" t="n">
         <v>0.0072</v>
       </c>
-      <c r="I20" s="8" t="n">
+      <c r="I20" s="7" t="n">
         <f aca="false">G20*H20</f>
         <v>10.8</v>
       </c>
@@ -1405,31 +1400,31 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10" t="n">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="E27" s="10" t="n">
+      <c r="E27" s="9" t="n">
         <v>0.1</v>
       </c>
-      <c r="F27" s="10" t="n">
+      <c r="F27" s="9" t="n">
         <f aca="false">D27*E27</f>
         <v>0</v>
       </c>
-      <c r="G27" s="10" t="n">
+      <c r="G27" s="9" t="n">
         <f aca="false">D27*500</f>
         <v>0</v>
       </c>
-      <c r="H27" s="10" t="n">
+      <c r="H27" s="9" t="n">
         <v>0.00405</v>
       </c>
-      <c r="I27" s="10" t="n">
+      <c r="I27" s="9" t="n">
         <f aca="false">G27*H27</f>
         <v>0</v>
       </c>
@@ -1499,46 +1494,44 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" s="10" t="n">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="E30" s="10" t="n">
+      <c r="E30" s="9" t="n">
         <v>1.2</v>
       </c>
-      <c r="F30" s="10" t="n">
+      <c r="F30" s="9" t="n">
         <f aca="false">D30*E30</f>
         <v>0</v>
       </c>
-      <c r="G30" s="10" t="n">
+      <c r="G30" s="9" t="n">
         <f aca="false">D30*500</f>
         <v>0</v>
       </c>
-      <c r="H30" s="10" t="n">
+      <c r="H30" s="9" t="n">
         <v>0.69894</v>
       </c>
-      <c r="I30" s="10" t="n">
+      <c r="I30" s="9" t="n">
         <f aca="false">G30*H30</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="D31" s="4" t="n">
         <v>2</v>
@@ -1562,131 +1555,129 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="10" t="n">
+      <c r="C32" s="9"/>
+      <c r="D32" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="E32" s="9" t="n">
+      <c r="E32" s="8" t="n">
         <v>2.64</v>
       </c>
-      <c r="F32" s="10" t="n">
+      <c r="F32" s="9" t="n">
         <f aca="false">E32*D32</f>
         <v>0</v>
       </c>
-      <c r="G32" s="9" t="n">
+      <c r="G32" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="H32" s="9" t="n">
+      <c r="H32" s="8" t="n">
         <v>1.5377</v>
       </c>
-      <c r="I32" s="10" t="n">
+      <c r="I32" s="9" t="n">
         <f aca="false">H32*G32</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D33" s="8" t="n">
+      <c r="D33" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="E33" s="11" t="n">
+      <c r="E33" s="10" t="n">
         <v>0.41</v>
       </c>
-      <c r="F33" s="12" t="n">
+      <c r="F33" s="11" t="n">
         <f aca="false">E33*D33</f>
         <v>0.41</v>
       </c>
-      <c r="G33" s="11" t="n">
+      <c r="G33" s="10" t="n">
         <v>500</v>
       </c>
-      <c r="H33" s="11" t="n">
+      <c r="H33" s="10" t="n">
         <v>0.15068</v>
       </c>
-      <c r="I33" s="12" t="n">
+      <c r="I33" s="11" t="n">
         <f aca="false">H33*G33</f>
         <v>75.34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="C34" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="D34" s="13" t="n">
+      <c r="D34" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="E34" s="13" t="n">
+      <c r="E34" s="12" t="n">
         <v>0.81</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">E34*D34</f>
         <v>0.81</v>
       </c>
-      <c r="G34" s="13" t="n">
+      <c r="G34" s="12" t="n">
         <v>500</v>
       </c>
-      <c r="H34" s="13" t="n">
+      <c r="H34" s="12" t="n">
         <v>0.33496</v>
       </c>
-      <c r="I34" s="12" t="n">
+      <c r="I34" s="11" t="n">
         <f aca="false">H34*G34</f>
         <v>167.48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
-      <c r="A35" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14" t="n">
+      <c r="A35" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13" t="n">
         <f aca="false">SUM(F2:F34)</f>
         <v>92.793</v>
       </c>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14" t="n">
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13" t="n">
         <f aca="false">SUM(I2:I34)/500</f>
         <v>44.23811</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
-      <c r="A37" s="14" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
+      <c r="A37" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
+      <c r="A38" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="0" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
-      <c r="A38" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B38" s="0" t="s">
+      <c r="C38" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>108</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>1</v>
@@ -1696,14 +1687,14 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="39">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B39" s="15" t="s">
-        <v>110</v>
-      </c>
       <c r="C39" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Worked a lot on layout and scematic for Rev A2
</commit_message>
<xml_diff>
--- a/PCB_rev1/Replicape_BOM_rev1.xlsx
+++ b/PCB_rev1/Replicape_BOM_rev1.xlsx
@@ -357,7 +357,6 @@
   <fonts count="5">
     <font>
       <name val="Verdana"/>
-      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -378,7 +377,6 @@
     </font>
     <font>
       <name val="Verdana"/>
-      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
@@ -562,14 +560,14 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+      <selection activeCell="C46" activeCellId="0" pane="topLeft" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.121568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.3254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7882352941176"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">

</xml_diff>